<commit_message>
and more notes on sampling methods
</commit_message>
<xml_diff>
--- a/vocabulary/IMLGSVocabularies.xlsx
+++ b/vocabulary/IMLGSVocabularies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/IEDA/vocabularies/vocabulary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smrTu\OneDrive\Documents\GithubC\IEDA\vocabularies\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{F5D3CE80-85FB-48BC-B932-09F62E79A31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{951974F2-4F84-4C27-8F82-E8B017715722}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBBCC79-44E1-4255-A5CA-55C429BD37B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="2370" windowWidth="12645" windowHeight="13740" xr2:uid="{40FB3A21-D53F-45A1-84E2-5B12BFCEC409}"/>
+    <workbookView xWindow="1837" yWindow="1657" windowWidth="17311" windowHeight="9143" xr2:uid="{40FB3A21-D53F-45A1-84E2-5B12BFCEC409}"/>
   </bookViews>
   <sheets>
     <sheet name="CollectionMethod" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="436">
   <si>
     <t>core, undifferentiated (0)</t>
   </si>
@@ -1367,13 +1367,31 @@
   </si>
   <si>
     <t>is there some fundamental difference in the sampling method with a giant (jumbo?) vs other piston coring</t>
+  </si>
+  <si>
+    <t>is this actually a different coring method, or just noting the instrument configuration?</t>
+  </si>
+  <si>
+    <t>what does this mean?  Drilling rock can be done lots of different ways, so this is a general category for any of those I assume</t>
+  </si>
+  <si>
+    <t>any coring method-- doesn't really specify a method, just that the product is core</t>
+  </si>
+  <si>
+    <t>I'm assumeing this is meant to include methods of sampling soft sediment with the various piston, gravity, box, vibrating … coring methods.  Have to be careful because connotation of drilling would not normally include those methods (IMO)</t>
+  </si>
+  <si>
+    <t>need definitons?  Probe coring?</t>
+  </si>
+  <si>
+    <t>devices aren't methods; they implement some method…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1502,10 +1520,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1827,17 +1841,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84575345-E70F-46D2-939E-AD148BAC63FE}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.4375" customWidth="1"/>
+    <col min="3" max="3" width="28.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1845,7 +1859,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1867,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1861,12 +1875,15 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1874,7 +1891,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1882,7 +1899,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1907,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1915,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1923,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1914,7 +1931,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1939,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1930,7 +1947,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +1955,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1946,7 +1963,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1954,15 +1971,18 @@
         <v>417</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1970,7 +1990,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1978,7 +1998,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1986,17 +2006,23 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2004,7 +2030,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2012,12 +2038,15 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +2054,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2033,7 +2062,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2041,12 +2070,15 @@
         <v>426</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>427</v>
+      </c>
+      <c r="D28" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2063,67 +2095,67 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="69.28515625" customWidth="1"/>
+    <col min="1" max="1" width="69.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="13.9">
       <c r="A1" s="15" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
         <v>405</v>
       </c>
@@ -2141,32 +2173,32 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="23.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2184,24 +2216,24 @@
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="1" max="1" width="20.5625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
@@ -2209,7 +2241,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
@@ -2217,7 +2249,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2225,7 +2257,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
@@ -2233,7 +2265,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
@@ -2241,7 +2273,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
@@ -2249,7 +2281,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
@@ -2257,7 +2289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
@@ -2265,7 +2297,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
@@ -2273,7 +2305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
@@ -2281,7 +2313,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" s="4" t="s">
         <v>44</v>
       </c>
@@ -2289,17 +2321,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
@@ -2307,7 +2339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
@@ -2315,7 +2347,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2323,12 +2355,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
@@ -2336,7 +2368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="4" t="s">
         <v>52</v>
       </c>
@@ -2344,12 +2376,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="4" t="s">
         <v>54</v>
       </c>
@@ -2357,7 +2389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="4" t="s">
         <v>55</v>
       </c>
@@ -2365,7 +2397,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="B25" s="4" t="s">
         <v>56</v>
       </c>
@@ -2373,7 +2405,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="B26" s="4" t="s">
         <v>57</v>
       </c>
@@ -2381,7 +2413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="B27" s="4" t="s">
         <v>58</v>
       </c>
@@ -2389,7 +2421,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
@@ -2397,7 +2429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" s="4" t="s">
         <v>60</v>
       </c>
@@ -2408,7 +2440,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
@@ -2416,7 +2448,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
@@ -2424,7 +2456,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
@@ -2432,12 +2464,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
@@ -2445,7 +2477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="B36" s="9" t="s">
         <v>82</v>
       </c>
@@ -2453,7 +2485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" s="9" t="s">
         <v>83</v>
       </c>
@@ -2461,7 +2493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" s="9" t="s">
         <v>84</v>
       </c>
@@ -2469,7 +2501,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" s="9" t="s">
         <v>85</v>
       </c>
@@ -2477,7 +2509,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" s="9" t="s">
         <v>86</v>
       </c>
@@ -2485,7 +2517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
@@ -2493,7 +2525,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="B42" s="9" t="s">
         <v>88</v>
       </c>
@@ -2501,7 +2533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="B43" s="9" t="s">
         <v>89</v>
       </c>
@@ -2509,7 +2541,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="B44" s="3"/>
     </row>
   </sheetData>
@@ -2525,13 +2557,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="29" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -2539,47 +2571,47 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
@@ -2597,222 +2629,222 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="32" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="7" t="s">
         <v>136</v>
       </c>
@@ -2830,255 +2862,255 @@
       <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="34.85546875" style="5" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
+    <col min="1" max="1" width="39.5625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="5"/>
+    <col min="3" max="3" width="34.875" style="5" customWidth="1"/>
+    <col min="4" max="5" width="9.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="C4" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="C5" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="C6" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="C7" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="C8" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="C9" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="C10" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="C11" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="C12" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="C13" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="C14" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="C15" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="C16" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="C17" s="14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="C18" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="C19" s="14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="C20" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="C21" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="C22" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="C23" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="C24" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="C25" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="C26" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="C27" s="14" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="C28" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="C29" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3">
       <c r="C30" s="14" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3">
       <c r="B32" s="14" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" s="14" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3">
       <c r="C34" s="14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3">
       <c r="C35" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3">
       <c r="C36" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3">
       <c r="C37" s="14" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3">
       <c r="C38" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3">
       <c r="C39" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3">
       <c r="C40" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3">
       <c r="C41" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3">
       <c r="C42" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3">
       <c r="C43" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3">
       <c r="C44" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3">
       <c r="C45" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3">
       <c r="C46" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3">
       <c r="C47" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3">
       <c r="C48" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6">
       <c r="C49" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6">
       <c r="B50" s="14" t="s">
         <v>186</v>
       </c>
@@ -3087,7 +3119,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="12"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6">
       <c r="B51" s="14"/>
       <c r="C51" s="14" t="s">
         <v>187</v>
@@ -3096,7 +3128,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6">
       <c r="B52" s="14"/>
       <c r="C52" s="14" t="s">
         <v>188</v>
@@ -3105,7 +3137,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6">
       <c r="B53" s="14"/>
       <c r="C53" s="14" t="s">
         <v>189</v>
@@ -3114,7 +3146,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6">
       <c r="B54" s="14"/>
       <c r="D54" s="14" t="s">
         <v>190</v>
@@ -3122,7 +3154,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6">
       <c r="B55" s="14"/>
       <c r="D55" s="14" t="s">
         <v>191</v>
@@ -3130,7 +3162,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6">
       <c r="B56" s="14"/>
       <c r="D56" s="14" t="s">
         <v>192</v>
@@ -3138,7 +3170,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6">
       <c r="B57" s="14"/>
       <c r="D57" s="14" t="s">
         <v>193</v>
@@ -3146,7 +3178,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6">
       <c r="B58" s="14"/>
       <c r="D58" s="14" t="s">
         <v>194</v>
@@ -3154,7 +3186,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6">
       <c r="B59" s="14"/>
       <c r="D59" s="14" t="s">
         <v>195</v>
@@ -3162,7 +3194,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6">
       <c r="B60" s="14"/>
       <c r="D60" s="14" t="s">
         <v>196</v>
@@ -3170,7 +3202,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="12"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6">
       <c r="B61" s="14"/>
       <c r="D61" s="14" t="s">
         <v>197</v>
@@ -3178,7 +3210,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6">
       <c r="B62" s="14"/>
       <c r="D62" s="14" t="s">
         <v>198</v>
@@ -3186,7 +3218,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6">
       <c r="B63" s="14"/>
       <c r="D63" s="14" t="s">
         <v>199</v>
@@ -3194,7 +3226,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="12"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6">
       <c r="B64" s="14"/>
       <c r="C64" s="14" t="s">
         <v>200</v>
@@ -3203,7 +3235,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="B65" s="14"/>
       <c r="C65" s="14" t="s">
         <v>201</v>
@@ -3212,7 +3244,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="B66" s="14"/>
       <c r="C66" s="14" t="s">
         <v>202</v>
@@ -3221,7 +3253,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="12"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="B67" s="14"/>
       <c r="C67" s="14" t="s">
         <v>203</v>
@@ -3230,7 +3262,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="12"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="B68" s="14"/>
       <c r="C68" s="14" t="s">
         <v>204</v>
@@ -3239,7 +3271,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="12"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="B69" s="14"/>
       <c r="C69" s="14" t="s">
         <v>205</v>
@@ -3248,7 +3280,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="12"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="B70" s="14"/>
       <c r="C70" s="14" t="s">
         <v>206</v>
@@ -3257,7 +3289,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="12"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="B71" s="14"/>
       <c r="C71" s="14" t="s">
         <v>207</v>
@@ -3266,7 +3298,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="12"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="B72" s="14"/>
       <c r="C72" s="14" t="s">
         <v>208</v>
@@ -3275,7 +3307,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="12"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="B73" s="14"/>
       <c r="C73" s="14" t="s">
         <v>209</v>
@@ -3284,7 +3316,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="B74" s="14"/>
       <c r="C74" s="14" t="s">
         <v>210</v>
@@ -3293,7 +3325,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="12"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="B75" s="14"/>
       <c r="D75" s="14" t="s">
         <v>211</v>
@@ -3301,7 +3333,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="B76" s="14"/>
       <c r="C76" s="14" t="s">
         <v>212</v>
@@ -3310,7 +3342,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="B77" s="14"/>
       <c r="C77" s="14" t="s">
         <v>213</v>
@@ -3319,7 +3351,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="12"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="B78" s="14"/>
       <c r="C78" s="14" t="s">
         <v>214</v>
@@ -3328,7 +3360,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="12"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="13" t="s">
         <v>215</v>
       </c>
@@ -3337,7 +3369,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="12"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="B80" s="14" t="s">
         <v>216</v>
       </c>
@@ -3346,7 +3378,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="12"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6">
       <c r="B81" s="14"/>
       <c r="C81" s="14" t="s">
         <v>217</v>
@@ -3355,7 +3387,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6">
       <c r="B82" s="14"/>
       <c r="C82" s="14" t="s">
         <v>218</v>
@@ -3364,7 +3396,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="12"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6">
       <c r="B83" s="14"/>
       <c r="C83" s="14" t="s">
         <v>219</v>
@@ -3373,7 +3405,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="12"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6">
       <c r="B84" s="14"/>
       <c r="C84" s="14" t="s">
         <v>220</v>
@@ -3382,7 +3414,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6">
       <c r="B85" s="14"/>
       <c r="C85" s="14" t="s">
         <v>221</v>
@@ -3391,7 +3423,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6">
       <c r="B86" s="14"/>
       <c r="C86" s="14" t="s">
         <v>222</v>
@@ -3400,7 +3432,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6">
       <c r="B87" s="14"/>
       <c r="C87" s="14" t="s">
         <v>223</v>
@@ -3409,7 +3441,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6">
       <c r="B88" s="14"/>
       <c r="C88" s="14" t="s">
         <v>224</v>
@@ -3418,7 +3450,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6">
       <c r="B89" s="14"/>
       <c r="C89" s="14" t="s">
         <v>225</v>
@@ -3427,7 +3459,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6">
       <c r="B90" s="14"/>
       <c r="C90" s="14" t="s">
         <v>226</v>
@@ -3436,7 +3468,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="12"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6">
       <c r="B91" s="14"/>
       <c r="C91" s="14" t="s">
         <v>227</v>
@@ -3445,352 +3477,352 @@
       <c r="E91" s="14"/>
       <c r="F91" s="12"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6">
       <c r="B92" s="14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6">
       <c r="C93" s="14" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6">
       <c r="C94" s="14" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6">
       <c r="C95" s="14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6">
       <c r="C96" s="14" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3">
       <c r="C97" s="14" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3">
       <c r="C98" s="14" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3">
       <c r="C99" s="14" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3">
       <c r="C100" s="14" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3">
       <c r="C101" s="14" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3">
       <c r="C102" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3">
       <c r="C103" s="14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3">
       <c r="C104" s="14" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3">
       <c r="C105" s="14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3">
       <c r="C106" s="14" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3">
       <c r="C107" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3">
       <c r="C108" s="14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3">
       <c r="C109" s="14" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3">
       <c r="C110" s="14" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3">
       <c r="C111" s="14" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3">
       <c r="C112" s="14" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="C113" s="14" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="C114" s="14" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="C115" s="14" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="C116" s="14" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="C117" s="14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="C118" s="14" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="C119" s="14" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3">
       <c r="B120" s="14" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3">
       <c r="C121" s="14" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3">
       <c r="C122" s="14" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3">
       <c r="C123" s="14" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3">
       <c r="C124" s="14" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3">
       <c r="C125" s="14" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3">
       <c r="C126" s="14" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3">
       <c r="C127" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3">
       <c r="C128" s="14" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3">
       <c r="C129" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3">
       <c r="C130" s="14" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3">
       <c r="C131" s="14" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3">
       <c r="C132" s="14" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3">
       <c r="C133" s="14" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3">
       <c r="C134" s="14" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3">
       <c r="C135" s="14" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3">
       <c r="C136" s="14" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3">
       <c r="C137" s="14" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3">
       <c r="C138" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3">
       <c r="C139" s="14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3">
       <c r="C140" s="14" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3">
       <c r="C141" s="14" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3">
       <c r="C142" s="14" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3">
       <c r="C143" s="14" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3">
       <c r="C144" s="14" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="B145" s="14" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="C146" s="14" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="C147" s="14" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="C148" s="14" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="C149" s="14" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="C150" s="14" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="C151" s="14" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="C152" s="14" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="C153" s="14" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="C154" s="14" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="C155" s="14" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="C156" s="14" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="C157" s="14" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="C158" s="14" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" s="13" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" s="14" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
         <v>322</v>
       </c>
@@ -3798,7 +3830,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" s="5" t="s">
         <v>322</v>
       </c>
@@ -3806,7 +3838,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" s="5" t="s">
         <v>322</v>
       </c>
@@ -3814,7 +3846,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" s="5" t="s">
         <v>322</v>
       </c>
@@ -3822,7 +3854,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" s="5" t="s">
         <v>322</v>
       </c>
@@ -3830,7 +3862,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
         <v>322</v>
       </c>
@@ -3838,7 +3870,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
         <v>322</v>
       </c>
@@ -3846,7 +3878,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3">
       <c r="A168" s="5" t="s">
         <v>322</v>
       </c>
@@ -3854,7 +3886,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
         <v>322</v>
       </c>
@@ -3862,7 +3894,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
         <v>322</v>
       </c>
@@ -3870,7 +3902,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
         <v>322</v>
       </c>
@@ -3878,7 +3910,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
         <v>322</v>
       </c>
@@ -3886,7 +3918,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
         <v>322</v>
       </c>
@@ -3894,7 +3926,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
         <v>322</v>
       </c>
@@ -3902,7 +3934,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
         <v>322</v>
       </c>
@@ -3910,7 +3942,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
         <v>322</v>
       </c>
@@ -3918,7 +3950,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2">
       <c r="A177" s="5" t="s">
         <v>322</v>
       </c>
@@ -3926,7 +3958,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2">
       <c r="A178" s="5" t="s">
         <v>322</v>
       </c>
@@ -3934,7 +3966,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2">
       <c r="A179" s="5" t="s">
         <v>322</v>
       </c>
@@ -3942,7 +3974,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2">
       <c r="A180" s="5" t="s">
         <v>322</v>
       </c>
@@ -3950,7 +3982,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2">
       <c r="A181" s="5" t="s">
         <v>322</v>
       </c>
@@ -3958,7 +3990,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2">
       <c r="A182" s="5" t="s">
         <v>322</v>
       </c>
@@ -3966,7 +3998,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2">
       <c r="A183" s="5" t="s">
         <v>322</v>
       </c>
@@ -3974,7 +4006,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2">
       <c r="A184" s="5" t="s">
         <v>322</v>
       </c>
@@ -3982,7 +4014,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2">
       <c r="A185" s="5" t="s">
         <v>322</v>
       </c>
@@ -3990,20 +4022,20 @@
         <v>347</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2">
       <c r="B186" s="14"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2">
       <c r="A187" s="13" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2">
       <c r="A188" s="14" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2">
       <c r="A189" s="5" t="s">
         <v>299</v>
       </c>
@@ -4011,7 +4043,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2">
       <c r="A190" s="5" t="s">
         <v>299</v>
       </c>
@@ -4019,7 +4051,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2">
       <c r="A191" s="5" t="s">
         <v>299</v>
       </c>
@@ -4027,7 +4059,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2">
       <c r="A192" s="5" t="s">
         <v>299</v>
       </c>
@@ -4035,7 +4067,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2">
       <c r="A193" s="5" t="s">
         <v>299</v>
       </c>
@@ -4043,7 +4075,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2">
       <c r="A194" s="5" t="s">
         <v>299</v>
       </c>
@@ -4051,7 +4083,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2">
       <c r="A195" s="5" t="s">
         <v>299</v>
       </c>
@@ -4059,7 +4091,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2">
       <c r="A196" s="5" t="s">
         <v>299</v>
       </c>
@@ -4067,7 +4099,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2">
       <c r="A197" s="5" t="s">
         <v>299</v>
       </c>
@@ -4075,7 +4107,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2">
       <c r="A198" s="5" t="s">
         <v>299</v>
       </c>
@@ -4083,7 +4115,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2">
       <c r="A199" s="5" t="s">
         <v>299</v>
       </c>
@@ -4091,7 +4123,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2">
       <c r="A200" s="5" t="s">
         <v>299</v>
       </c>
@@ -4099,10 +4131,10 @@
         <v>316</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2">
       <c r="B201" s="14"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2">
       <c r="A202" s="5" t="s">
         <v>321</v>
       </c>
@@ -4110,7 +4142,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2">
       <c r="A203" s="5" t="s">
         <v>321</v>
       </c>
@@ -4118,7 +4150,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2">
       <c r="A204" s="5" t="s">
         <v>321</v>
       </c>
@@ -4126,7 +4158,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2">
       <c r="A205" s="5" t="s">
         <v>321</v>
       </c>
@@ -4134,7 +4166,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2">
       <c r="A206" s="5" t="s">
         <v>321</v>
       </c>
@@ -4142,7 +4174,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2">
       <c r="A207" s="5" t="s">
         <v>321</v>
       </c>
@@ -4150,7 +4182,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2">
       <c r="A208" s="5" t="s">
         <v>321</v>
       </c>
@@ -4158,7 +4190,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2">
       <c r="A209" s="5" t="s">
         <v>321</v>
       </c>
@@ -4166,7 +4198,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2">
       <c r="A210" s="5" t="s">
         <v>321</v>
       </c>
@@ -4187,169 +4219,169 @@
       <selection activeCell="B28" sqref="B28:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="29" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.4375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="B3" s="14" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="B4" s="14" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="B5" s="14" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" s="14" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="B7" s="14" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="B8" s="14" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="B9" s="14" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="14" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="B11" s="14" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="B12" s="14" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="B13" s="14" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="B14" s="14" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="14" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="B16" s="14" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="B17" s="14" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="B18" s="14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="B19" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="B20" s="14" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="14" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="B22" s="14" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="B23" s="14" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="B24" s="14" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="B25" s="14" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="B26" s="14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="14" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="B28" s="14" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="B29" s="14" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="B30" s="14" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" s="14" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="B32" s="14" t="s">
         <v>379</v>
       </c>
@@ -4367,65 +4399,65 @@
       <selection activeCell="A8" sqref="A8:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="11" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="11" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="11"/>
     </row>
   </sheetData>
@@ -4441,42 +4473,42 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="3" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" s="3" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" s="3" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" s="3" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" s="3" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" s="3" customFormat="1">
       <c r="A6" s="4" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
         <v>392</v>
       </c>

</xml_diff>

<commit_message>
updating vocabularies for sesar mapping
</commit_message>
<xml_diff>
--- a/vocabulary/IMLGSVocabularies.xlsx
+++ b/vocabulary/IMLGSVocabularies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smrTu\OneDrive\Documents\GithubC\IEDA\vocabularies\vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/IEDA/vocabularies/vocabulary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBBCC79-44E1-4255-A5CA-55C429BD37B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2DBBCC79-44E1-4255-A5CA-55C429BD37B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB9B1194-D290-4371-A334-B51082D7619A}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1657" windowWidth="17311" windowHeight="9143" xr2:uid="{40FB3A21-D53F-45A1-84E2-5B12BFCEC409}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="25800" windowHeight="13440" activeTab="5" xr2:uid="{40FB3A21-D53F-45A1-84E2-5B12BFCEC409}"/>
   </bookViews>
   <sheets>
     <sheet name="CollectionMethod" sheetId="1" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1841,17 +1841,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84575345-E70F-46D2-939E-AD148BAC63FE}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.4375" customWidth="1"/>
-    <col min="3" max="3" width="28.4375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2095,67 +2095,67 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.3125" customWidth="1"/>
+    <col min="1" max="1" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13.9">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>405</v>
       </c>
@@ -2173,32 +2173,32 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.3125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="23.25">
+    <row r="5" spans="1:1" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2216,24 +2216,24 @@
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="3"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>44</v>
       </c>
@@ -2321,17 +2321,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2355,12 +2355,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>52</v>
       </c>
@@ -2376,12 +2376,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>54</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>55</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>56</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>57</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>58</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>60</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
@@ -2464,12 +2464,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
         <v>82</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
         <v>83</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
         <v>84</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>85</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>86</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
         <v>88</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>89</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
     </row>
   </sheetData>
@@ -2557,13 +2557,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.5625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -2571,47 +2571,47 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
@@ -2629,222 +2629,222 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>136</v>
       </c>
@@ -2858,259 +2858,259 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0585861F-0F2C-4D53-B3EC-46E5ECDFA86F}">
   <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
       <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="5"/>
-    <col min="3" max="3" width="34.875" style="5" customWidth="1"/>
-    <col min="4" max="5" width="9.125" style="5"/>
+    <col min="1" max="1" width="39.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="58" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="5" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" s="14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" s="14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" s="14" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="14" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="14" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="3:3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="3:3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="3:3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="3:3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="3:3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="3:3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C49" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
         <v>186</v>
       </c>
@@ -3119,7 +3119,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="12"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="14"/>
       <c r="C51" s="14" t="s">
         <v>187</v>
@@ -3128,7 +3128,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
       <c r="C52" s="14" t="s">
         <v>188</v>
@@ -3137,7 +3137,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
       <c r="C53" s="14" t="s">
         <v>189</v>
@@ -3146,7 +3146,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="D54" s="14" t="s">
         <v>190</v>
@@ -3154,7 +3154,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
       <c r="D55" s="14" t="s">
         <v>191</v>
@@ -3162,7 +3162,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
       <c r="D56" s="14" t="s">
         <v>192</v>
@@ -3170,7 +3170,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
       <c r="D57" s="14" t="s">
         <v>193</v>
@@ -3178,7 +3178,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="14"/>
       <c r="D58" s="14" t="s">
         <v>194</v>
@@ -3186,7 +3186,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
       <c r="D59" s="14" t="s">
         <v>195</v>
@@ -3194,7 +3194,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
       <c r="D60" s="14" t="s">
         <v>196</v>
@@ -3202,7 +3202,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="12"/>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="14"/>
       <c r="D61" s="14" t="s">
         <v>197</v>
@@ -3210,7 +3210,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="14"/>
       <c r="D62" s="14" t="s">
         <v>198</v>
@@ -3218,7 +3218,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="14"/>
       <c r="D63" s="14" t="s">
         <v>199</v>
@@ -3226,7 +3226,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="12"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
       <c r="C64" s="14" t="s">
         <v>200</v>
@@ -3235,7 +3235,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
       <c r="C65" s="14" t="s">
         <v>201</v>
@@ -3244,7 +3244,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="C66" s="14" t="s">
         <v>202</v>
@@ -3253,7 +3253,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="12"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" s="14"/>
       <c r="C67" s="14" t="s">
         <v>203</v>
@@ -3262,7 +3262,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="12"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" s="14"/>
       <c r="C68" s="14" t="s">
         <v>204</v>
@@ -3271,7 +3271,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="12"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="14"/>
       <c r="C69" s="14" t="s">
         <v>205</v>
@@ -3280,7 +3280,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="12"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="14"/>
       <c r="C70" s="14" t="s">
         <v>206</v>
@@ -3289,7 +3289,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="12"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="14" t="s">
         <v>207</v>
@@ -3298,7 +3298,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="12"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="14"/>
       <c r="C72" s="14" t="s">
         <v>208</v>
@@ -3307,7 +3307,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="12"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="14"/>
       <c r="C73" s="14" t="s">
         <v>209</v>
@@ -3316,7 +3316,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" s="14"/>
       <c r="C74" s="14" t="s">
         <v>210</v>
@@ -3325,7 +3325,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="12"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="14"/>
       <c r="D75" s="14" t="s">
         <v>211</v>
@@ -3333,7 +3333,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="14"/>
       <c r="C76" s="14" t="s">
         <v>212</v>
@@ -3342,7 +3342,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="14"/>
       <c r="C77" s="14" t="s">
         <v>213</v>
@@ -3351,7 +3351,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="12"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="14"/>
       <c r="C78" s="14" t="s">
         <v>214</v>
@@ -3360,7 +3360,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="12"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>215</v>
       </c>
@@ -3369,7 +3369,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="12"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
         <v>216</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="12"/>
     </row>
-    <row r="81" spans="2:6">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="14"/>
       <c r="C81" s="14" t="s">
         <v>217</v>
@@ -3387,7 +3387,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="2:6">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="14"/>
       <c r="C82" s="14" t="s">
         <v>218</v>
@@ -3396,7 +3396,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="12"/>
     </row>
-    <row r="83" spans="2:6">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="14"/>
       <c r="C83" s="14" t="s">
         <v>219</v>
@@ -3405,7 +3405,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="12"/>
     </row>
-    <row r="84" spans="2:6">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="14"/>
       <c r="C84" s="14" t="s">
         <v>220</v>
@@ -3414,7 +3414,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="2:6">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="14"/>
       <c r="C85" s="14" t="s">
         <v>221</v>
@@ -3423,7 +3423,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="2:6">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="14"/>
       <c r="C86" s="14" t="s">
         <v>222</v>
@@ -3432,7 +3432,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="2:6">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="14"/>
       <c r="C87" s="14" t="s">
         <v>223</v>
@@ -3441,7 +3441,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="2:6">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="14"/>
       <c r="C88" s="14" t="s">
         <v>224</v>
@@ -3450,7 +3450,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="2:6">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="14"/>
       <c r="C89" s="14" t="s">
         <v>225</v>
@@ -3459,7 +3459,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="2:6">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="14"/>
       <c r="C90" s="14" t="s">
         <v>226</v>
@@ -3468,7 +3468,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="12"/>
     </row>
-    <row r="91" spans="2:6">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="14"/>
       <c r="C91" s="14" t="s">
         <v>227</v>
@@ -3477,352 +3477,352 @@
       <c r="E91" s="14"/>
       <c r="F91" s="12"/>
     </row>
-    <row r="92" spans="2:6">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="2:6">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C93" s="14" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="2:6">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C94" s="14" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="2:6">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C95" s="14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="96" spans="2:6">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C96" s="14" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="97" spans="3:3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="14" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="14" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="14" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="14" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="14" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="102" spans="3:3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="14" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="14" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="107" spans="3:3">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="108" spans="3:3">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="109" spans="3:3">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="14" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="3:3">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="14" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="111" spans="3:3">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="14" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="112" spans="3:3">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="14" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C113" s="14" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C114" s="14" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C115" s="14" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C116" s="14" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C117" s="14" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C118" s="14" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C119" s="14" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C121" s="14" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C122" s="14" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C123" s="14" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="124" spans="2:3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C124" s="14" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="125" spans="2:3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C125" s="14" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="126" spans="2:3">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C126" s="14" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="127" spans="2:3">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C127" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="128" spans="2:3">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C128" s="14" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="129" spans="3:3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="130" spans="3:3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="14" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="14" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="132" spans="3:3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="14" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="3:3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="14" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="134" spans="3:3">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="14" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="135" spans="3:3">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="14" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="136" spans="3:3">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="14" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="137" spans="3:3">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="14" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="3:3">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="139" spans="3:3">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="140" spans="3:3">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="14" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="3:3">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="14" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="142" spans="3:3">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="14" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="3:3">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="14" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="144" spans="3:3">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="14" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C146" s="14" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C147" s="14" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C148" s="14" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C149" s="14" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C150" s="14" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C151" s="14" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C152" s="14" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C153" s="14" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C154" s="14" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C155" s="14" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C156" s="14" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C157" s="14" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C158" s="14" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>322</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>322</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>322</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>322</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>322</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>322</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>322</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>322</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>322</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>322</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>322</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>322</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>322</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>322</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>322</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>322</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>322</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>322</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>322</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>322</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>322</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>322</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>322</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>322</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>322</v>
       </c>
@@ -4022,20 +4022,20 @@
         <v>347</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B186" s="14"/>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="13" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>299</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>299</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>299</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>299</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>299</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>299</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>299</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>299</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>299</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>299</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>299</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>299</v>
       </c>
@@ -4131,10 +4131,10 @@
         <v>316</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B201" s="14"/>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>321</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>321</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>321</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>321</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>321</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>321</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>321</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>321</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>321</v>
       </c>
@@ -4219,169 +4219,169 @@
       <selection activeCell="B28" sqref="B28:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.4375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>379</v>
       </c>
@@ -4399,65 +4399,65 @@
       <selection activeCell="A8" sqref="A8:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.3125" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
     </row>
   </sheetData>
@@ -4473,42 +4473,42 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.4375" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1">
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="3" customFormat="1">
+    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="3" customFormat="1">
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="3" customFormat="1">
+    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="3" customFormat="1">
+    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="3" customFormat="1">
+    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>392</v>
       </c>

</xml_diff>